<commit_message>
Seguimos con el analisis de las series del primer parcial
</commit_message>
<xml_diff>
--- a/Accidentes_transito_full.xlsx
+++ b/Accidentes_transito_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9e6e0322c927b48/Documentos/MIS_UNAM/Segundo_semestre/Series_UNAM_HPi3/Series_UNAM_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{DA11D808-633B-46A4-AA40-571C6C221D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5AD66FD-1AB1-4040-92D1-0FF8DD77D14E}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{DA11D808-633B-46A4-AA40-571C6C221D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD88A24-AE58-4C1C-81E7-5A74E3A5378E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9C482A4-B857-436F-9DC5-C4D7D20035FB}"/>
   </bookViews>
@@ -96,6 +96,1022 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Accidentes_MEX!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>36537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37633</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38364</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39459</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39825</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40555</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40920</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41286</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41651</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42747</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43112</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43477</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43842</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Accidentes_MEX!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>311938</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>364869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>399002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>424940</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>443607</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>452233</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>471272</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>476279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>466435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>428467</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>427267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>387185</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>390411</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>385772</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>380573</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>382066</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>360051</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>367789</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>365281</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>362729</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>301068</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>340415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA98-4941-8056-FB562B1138D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="117875808"/>
+        <c:axId val="117868128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="117875808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="117868128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="117868128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="117875808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86EBD2C9-B881-11DB-B07F-DE98DE98D358}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,18 +1415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56C9B97-9B1C-404C-8FDA-8FD68F7658A2}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>36537</v>
       </c>
@@ -426,7 +1444,7 @@
         <v>311938</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>36903</v>
       </c>
@@ -434,7 +1452,7 @@
         <v>364869</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>37268</v>
       </c>
@@ -442,15 +1460,18 @@
         <v>399002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>37633</v>
       </c>
       <c r="B5" s="2">
         <v>424940</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="2">
+        <v>424940</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>37998</v>
       </c>
@@ -458,7 +1479,7 @@
         <v>443607</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>38364</v>
       </c>
@@ -466,7 +1487,7 @@
         <v>452233</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>38729</v>
       </c>
@@ -474,7 +1495,7 @@
         <v>471272</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>39094</v>
       </c>
@@ -482,7 +1503,7 @@
         <v>476279</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>39459</v>
       </c>
@@ -490,7 +1511,7 @@
         <v>466435</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>39825</v>
       </c>
@@ -498,7 +1519,7 @@
         <v>428467</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>40190</v>
       </c>
@@ -506,7 +1527,7 @@
         <v>427267</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>40555</v>
       </c>
@@ -514,7 +1535,7 @@
         <v>387185</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>40920</v>
       </c>
@@ -522,7 +1543,7 @@
         <v>390411</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>41286</v>
       </c>
@@ -530,7 +1551,7 @@
         <v>385772</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>41651</v>
       </c>
@@ -796,5 +1817,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>